<commit_message>
Finished most functionality in hoard table rolls, updated readme
</commit_message>
<xml_diff>
--- a/individual_items.xlsx
+++ b/individual_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8864B73-B875-41D9-954D-DD68263E004A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28171A-D45B-46ED-9B5B-AFA3F44AAA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="653" xr2:uid="{EB3FE16E-157E-4914-A7D1-6C101C7199CA}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="669">
   <si>
     <t>Armor, +3 plate</t>
   </si>
@@ -2485,7 +2485,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2497,6 +2497,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>653</v>
+      </c>
       <c r="B1">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Finished functionality for hoard_reward_roll.py. all items are properly fetched
</commit_message>
<xml_diff>
--- a/individual_items.xlsx
+++ b/individual_items.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28171A-D45B-46ED-9B5B-AFA3F44AAA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668B6BDE-D388-4FD4-9130-EE93C17EF32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="653" xr2:uid="{EB3FE16E-157E-4914-A7D1-6C101C7199CA}"/>
+    <workbookView xWindow="57480" yWindow="16230" windowWidth="25440" windowHeight="15390" tabRatio="653" activeTab="6" xr2:uid="{EB3FE16E-157E-4914-A7D1-6C101C7199CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Art Objects" sheetId="7" r:id="rId1"/>
     <sheet name="Gems" sheetId="6" r:id="rId2"/>
     <sheet name="Ammunition" sheetId="5" r:id="rId3"/>
     <sheet name="Weapons" sheetId="4" r:id="rId4"/>
-    <sheet name="Armor Type" sheetId="3" r:id="rId5"/>
+    <sheet name="Armor" sheetId="3" r:id="rId5"/>
     <sheet name="Magic Armor" sheetId="2" r:id="rId6"/>
-    <sheet name="Figureine of Wondrous Power" sheetId="8" r:id="rId7"/>
+    <sheet name="Figurine of Wondrous Power" sheetId="8" r:id="rId7"/>
     <sheet name="Cantrips" sheetId="23" r:id="rId8"/>
     <sheet name="Level 1" sheetId="11" r:id="rId9"/>
     <sheet name="Level 2" sheetId="13" r:id="rId10"/>
@@ -2483,7 +2483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85B3EE1-6AFF-4A57-8DA1-7E554C0976DB}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -3344,7 +3344,1276 @@
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="5"/>
+    <col min="2" max="2" width="23.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="10"/>
+    <col min="4" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+    </row>
+    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+    </row>
+    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+    </row>
+    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+    </row>
+    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+    </row>
+    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+    </row>
+    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+    </row>
+    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C81" s="8"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+    </row>
+    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4B38CB-D9E1-40A3-858B-D2FB55163BFE}">
+  <dimension ref="A1:I73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C40" sqref="C40"/>
       <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
@@ -3377,1275 +4646,6 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="5">
-        <v>31</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="5">
-        <v>32</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="5">
-        <v>33</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="5">
-        <v>34</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="5">
-        <v>36</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="5">
-        <v>37</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="5">
-        <v>38</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="5">
-        <v>39</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="5">
-        <v>40</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="5">
-        <v>41</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="5">
-        <v>42</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="5">
-        <v>43</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="5">
-        <v>44</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="5">
-        <v>45</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="5">
-        <v>46</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="5">
-        <v>47</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="5">
-        <v>48</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="5">
-        <v>49</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-    </row>
-    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="5">
-        <v>50</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-    </row>
-    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="5">
-        <v>51</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-    </row>
-    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="5">
-        <v>52</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-    </row>
-    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="5">
-        <v>53</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-    </row>
-    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="5">
-        <v>54</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-    </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="5">
-        <v>55</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-    </row>
-    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="5">
-        <v>56</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-    </row>
-    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="5">
-        <v>57</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-    </row>
-    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="5">
-        <v>58</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-    </row>
-    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="5">
-        <v>59</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-    </row>
-    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="5">
-        <v>60</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-    </row>
-    <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="5">
-        <v>61</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-    </row>
-    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="5">
-        <v>62</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-    </row>
-    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="5">
-        <v>63</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-    </row>
-    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="5">
-        <v>64</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-    </row>
-    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="5">
-        <v>65</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-    </row>
-    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="5">
-        <v>66</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-    </row>
-    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="5">
-        <v>67</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-    </row>
-    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="5">
-        <v>68</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
-    </row>
-    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="5">
-        <v>69</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-    </row>
-    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="5">
-        <v>70</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
-    </row>
-    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="5">
-        <v>71</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
-    </row>
-    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="5">
-        <v>72</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
-    </row>
-    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="5">
-        <v>73</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="5">
-        <v>74</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-    </row>
-    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="5">
-        <v>75</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-    </row>
-    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="5">
-        <v>76</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="5">
-        <v>77</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-    </row>
-    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="5">
-        <v>78</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="5">
-        <v>79</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C80" s="8"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
-    </row>
-    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="5">
-        <v>80</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-    </row>
-    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="5">
-        <v>81</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C82" s="8"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
-    </row>
-    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="5">
-        <v>82</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4B38CB-D9E1-40A3-858B-D2FB55163BFE}">
-  <dimension ref="A1:I73"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="C40" sqref="C40"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="5"/>
-    <col min="2" max="2" width="19.90625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="10"/>
-    <col min="4" max="16384" width="8.7265625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
         <v>367</v>
       </c>
       <c r="C2" s="8"/>
@@ -5732,7 +5732,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C40" sqref="C40"/>
       <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
@@ -6581,7 +6581,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C40" sqref="C40"/>
       <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
@@ -12939,7 +12939,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13199,9 +13199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C89054-848B-4DFC-A312-8742A137501D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13296,7 +13296,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F60"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>